<commit_message>
Correcting the issue with missing keys in incidences. Still in progress.
- Added default incidences in load_incidencias to handle missing keys.
- Updated TicketManagement to ensure it can handle missing keys in incidences.
- Modified beta_version.py to properly load and pass incidences to TicketManagement.

This commit addresses the problem where incidences keys were missing and causing KeyError.
Still working on the permanent fix for the admin changes not persisting across sessions.
</commit_message>
<xml_diff>
--- a/beta_version/excel_files/test.xlsx
+++ b/beta_version/excel_files/test.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -590,6 +590,38 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>WV50 FILTER</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Cover atascasdo</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>2024-06-26</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>12:50:14</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>-0.01 minutos</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>